<commit_message>
- added some lines at YOLOv3 text
</commit_message>
<xml_diff>
--- a/Tabellen/Objecte in Buero.xlsx
+++ b/Tabellen/Objecte in Buero.xlsx
@@ -10,6 +10,9 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$AT:$AT</definedName>
+  </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -20,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="68">
   <si>
     <t xml:space="preserve">Büro</t>
   </si>
@@ -221,6 +224,9 @@
   </si>
   <si>
     <t xml:space="preserve">mobilephone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sa</t>
   </si>
 </sst>
 </file>
@@ -396,15 +402,19 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AN57"/>
+  <dimension ref="A1:AT57"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I16" activeCellId="0" sqref="I16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AE1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AM27" activeCellId="0" sqref="AM27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -527,6 +537,9 @@
       <c r="AN1" s="0" t="n">
         <v>-0.004</v>
       </c>
+      <c r="AT1" s="0" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
@@ -643,6 +656,9 @@
       <c r="AN2" s="0" t="n">
         <v>0.004</v>
       </c>
+      <c r="AT2" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
@@ -759,6 +775,9 @@
       <c r="AN3" s="0" t="n">
         <v>0.031</v>
       </c>
+      <c r="AT3" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
@@ -875,6 +894,9 @@
       <c r="AN4" s="0" t="n">
         <v>0.043</v>
       </c>
+      <c r="AT4" s="0" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
@@ -991,6 +1013,9 @@
       <c r="AN5" s="0" t="n">
         <v>0.045</v>
       </c>
+      <c r="AT5" s="0" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
@@ -1107,6 +1132,9 @@
       <c r="AN6" s="0" t="n">
         <v>0.047</v>
       </c>
+      <c r="AT6" s="0" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
@@ -1223,6 +1251,9 @@
       <c r="AN7" s="0" t="n">
         <v>0.05</v>
       </c>
+      <c r="AT7" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
@@ -1339,6 +1370,9 @@
       <c r="AN8" s="0" t="n">
         <v>0.083</v>
       </c>
+      <c r="AT8" s="0" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
@@ -1455,6 +1489,9 @@
       <c r="AN9" s="0" t="n">
         <v>0.089</v>
       </c>
+      <c r="AT9" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
@@ -1571,6 +1608,9 @@
       <c r="AN10" s="0" t="n">
         <v>0.095</v>
       </c>
+      <c r="AT10" s="0" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
@@ -2186,6 +2226,9 @@
       <c r="B25" s="1" t="n">
         <v>0.106</v>
       </c>
+      <c r="C25" s="0" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
@@ -2194,6 +2237,9 @@
       <c r="B26" s="0" t="n">
         <v>0.121</v>
       </c>
+      <c r="C26" s="0" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
@@ -2202,6 +2248,9 @@
       <c r="B27" s="0" t="n">
         <v>0.158</v>
       </c>
+      <c r="C27" s="0" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
@@ -2210,6 +2259,9 @@
       <c r="B28" s="0" t="n">
         <v>0.18</v>
       </c>
+      <c r="C28" s="0" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
@@ -2218,6 +2270,9 @@
       <c r="B29" s="0" t="n">
         <v>0.195</v>
       </c>
+      <c r="C29" s="0" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
@@ -2226,6 +2281,9 @@
       <c r="B30" s="0" t="n">
         <v>0.198</v>
       </c>
+      <c r="C30" s="0" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
@@ -2234,6 +2292,9 @@
       <c r="B31" s="0" t="n">
         <v>0.223</v>
       </c>
+      <c r="C31" s="0" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
@@ -2241,6 +2302,9 @@
       </c>
       <c r="B32" s="0" t="n">
         <v>0.245</v>
+      </c>
+      <c r="C32" s="0" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2250,6 +2314,9 @@
       <c r="B33" s="0" t="n">
         <v>0.269</v>
       </c>
+      <c r="C33" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
@@ -2258,6 +2325,14 @@
       <c r="B34" s="0" t="n">
         <v>0.34</v>
       </c>
+      <c r="C34" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AP38" s="0" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AL49" s="0" t="s">
@@ -2332,6 +2407,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="AT:AT"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -2339,5 +2415,6 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>